<commit_message>
Fourth commit, Second rule metal spacing 1.2
</commit_message>
<xml_diff>
--- a/All_rules.xlsx
+++ b/All_rules.xlsx
@@ -36,8 +36,7 @@
     <t>rule METAL1.SP.1.1 {
     caption METAL1.SP.1.1: Metal1 to Metal1 spacing must be &gt;= 0.06 um;
     exte Metal1 Metal1 -lt 0.06 -output region -singular -abut lt 90;
-}
-</t>
+}</t>
   </si>
   <si>
     <t>METAL1.SP.1.2</t>
@@ -60,8 +59,7 @@
 }</t>
   </si>
   <si>
-    <t>drc = exte
-</t>
+    <t>drc = exte</t>
   </si>
 </sst>
 </file>
@@ -76,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,11 +96,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,6 +216,7 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="107.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
Incomplete lines are merged in the input file,written rule for METAL2.E.1
</commit_message>
<xml_diff>
--- a/All_rules.xlsx
+++ b/All_rules.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Rule</t>
   </si>
@@ -61,6 +61,54 @@
   <si>
     <t>drc = exte</t>
   </si>
+  <si>
+    <t>METAL3.E.1</t>
+  </si>
+  <si>
+    <t>L67626=geomAndNot(Via2 metal3_conn)
+errorLayer(L67626 "METAL3.E.1: Metal3 to Via2 enclosure must be &gt;= 0.005 um")
+L7300=drc(metal3_conn Via2 enc&lt;0.005)
+errorLayer(L7300 "METAL3.E.1: Metal3 to Via2 enclosure must be &gt;= 0.005 um")</t>
+  </si>
+  <si>
+    <t>rule METAL3.E.1 {
+    caption METAL3.E.1: Metal3 to Via2 enclosure must be &gt;= 0.005 um;
+    enc Via2 metal3_conn -lt 0.005 -output region -singular -abut lt 90 -outside_also;
+}</t>
+  </si>
+  <si>
+    <t>METAL1.E.1</t>
+  </si>
+  <si>
+    <t>L80230=geomAndNot(Cont metal1_conn)
+errorLayer(L80230 "METAL1.E.1: Metal1 to Cont enclosure must be &gt;= 0.00 um")</t>
+  </si>
+  <si>
+    <t>not Cont metal1_conn L24896;
+rule METAL1.E.1 {
+    caption METAL1.E.1: 0.00 &gt;= 0.00 um;
+    copy L24896;
+}
+</t>
+  </si>
+  <si>
+    <t>METAL2.E.1</t>
+  </si>
+  <si>
+    <t>L12682=geomAndNot(Via1 metal2_conn)
+errorLayer(L12682 "METAL2.E.1: Metal2 to Via1 enclosure must be &gt;= 0.005 um")
+L66270=drc(metal2_conn Via1 enc&lt;0.005)
+errorLayer(L66270 "METAL2.E.1: Metal2 to Via1 enclosure must be &gt;= 0.005 um")</t>
+  </si>
+  <si>
+    <t>rule METAL2.E.1 {
+    caption METAL2.E.1: Metal2 to Via1 enclosure must be &gt;= 0.005 um;
+    enc Via1 metal2_conn -lt 0.005 -output region -singular -abut lt 90 -outside_also;
+}</t>
+  </si>
+  <si>
+    <t>Have to process first 2 lines</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -103,6 +151,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -161,6 +214,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,16 +238,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="75.2602040816327"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5204081632653"/>
   </cols>
@@ -230,6 +287,42 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="72.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on rule for METAL1.W.1
</commit_message>
<xml_diff>
--- a/All_rules.xlsx
+++ b/All_rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="222" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Rule</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>PVL</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>METAL1.SP.1.1</t>
@@ -37,6 +40,9 @@
     caption METAL1.SP.1.1: Metal1 to Metal1 spacing must be &gt;= 0.06 um;
     exte Metal1 Metal1 -lt 0.06 -output region -singular -abut lt 90;
 }</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
   <si>
     <t>METAL1.SP.1.2</t>
@@ -59,7 +65,7 @@
 }</t>
   </si>
   <si>
-    <t>drc = exte</t>
+    <t>drc = exte size and edge boolean not printing outside the reule</t>
   </si>
   <si>
     <t>METAL3.E.1</t>
@@ -88,8 +94,7 @@
 rule METAL1.E.1 {
     caption METAL1.E.1: 0.00 &gt;= 0.00 um;
     copy L24896;
-}
-</t>
+}</t>
   </si>
   <si>
     <t>METAL2.E.1</t>
@@ -108,6 +113,45 @@
   </si>
   <si>
     <t>Have to process first 2 lines</t>
+  </si>
+  <si>
+    <t>METAL1.E.2</t>
+  </si>
+  <si>
+    <t>L89929=geomAnd(Cont metal1_conn)
+L83995=drc(metal1_conn L89929 venc(enc1&lt;0.06 enc2&lt;0 enc3&lt;0.06 enc4&lt;0))
+errorLayer(L83995
+    "METAL1.E.2: Metal1 to Cont enclosure on opposite sides must be &gt;= 0.06 um")
+</t>
+  </si>
+  <si>
+    <t>and Cont metal1_conn L83068;
+rule METAL1.E.2 {
+    caption METAL1.E.2: 0.03 &gt;= 0.03 um;
+    grow L83068 -left 0.03 -right 0.03 L52391;
+    select -inside L52391 metal1_conn L46178;
+    not L83068 L46178 L29812;
+    grow L29812 -top 0.03 -bottom 0.03 L21027;
+    select -inside L21027 metal1_conn L30406;
+    not L29812 L30406;
+}</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>METAL1.W.1</t>
+  </si>
+  <si>
+    <t>L91458=drc(metal1_conn width&lt;0.12)
+errorLayer(L91458 "METAL1.W.1: Metal1 width must be &gt;= 0.12 um")
+</t>
+  </si>
+  <si>
+    <t>rule METAL1.W.1 {
+    caption METAL1.W.1: Metal1 width must be &gt;= 0.06 um;
+    inte metal1_conn metal1_conn -lt 0.06 -output region -singular -abut lt 90;
+}</t>
   </si>
 </sst>
 </file>
@@ -200,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,6 +258,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,10 +290,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -252,7 +304,7 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -262,67 +314,101 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="60.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="107.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="72.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
+    </row>
+    <row r="5" customFormat="false" ht="60.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
+      <c r="A6" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on Oxide Rule,72 rules got completed
</commit_message>
<xml_diff>
--- a/All_rules.xlsx
+++ b/All_rules.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Rule</t>
   </si>
@@ -121,8 +121,7 @@
     <t>L89929=geomAnd(Cont metal1_conn)
 L83995=drc(metal1_conn L89929 venc(enc1&lt;0.06 enc2&lt;0 enc3&lt;0.06 enc4&lt;0))
 errorLayer(L83995
-    "METAL1.E.2: Metal1 to Cont enclosure on opposite sides must be &gt;= 0.06 um")
-</t>
+    "METAL1.E.2: Metal1 to Cont enclosure on opposite sides must be &gt;= 0.06 um")</t>
   </si>
   <si>
     <t>and Cont metal1_conn L83068;
@@ -144,13 +143,28 @@
   </si>
   <si>
     <t>L91458=drc(metal1_conn width&lt;0.12)
-errorLayer(L91458 "METAL1.W.1: Metal1 width must be &gt;= 0.12 um")
-</t>
+errorLayer(L91458 "METAL1.W.1: Metal1 width must be &gt;= 0.12 um")</t>
   </si>
   <si>
     <t>rule METAL1.W.1 {
     caption METAL1.W.1: Metal1 width must be &gt;= 0.06 um;
     inte metal1_conn metal1_conn -lt 0.06 -output region -singular -abut lt 90;
+}</t>
+  </si>
+  <si>
+    <t>OXIDE.W.2.1.2</t>
+  </si>
+  <si>
+    <t>L19348=geomAnd(L76283 Poly)
+L96558=geomGetEdge(Oxide inside L19348)
+L83789=drc(L96558 width&lt;0.15)
+errorLayer(L83789 "OXIDE.W.2.1.2: 2.5V N-channel gate width must be &gt;= 0.15 um")</t>
+  </si>
+  <si>
+    <t>
+rule OXIDE.W.2.1.2 {
+    caption OXIDE.W.2.1.2: Minimum 1.8V N-channel gate width &gt;= 0.32 um;
+    inte L43550 L43550 -lt 0.32 -output region -abut lt 90;
 }</t>
   </si>
 </sst>
@@ -290,16 +304,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="75.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.0969387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5204081632653"/>
   </cols>
@@ -370,7 +386,9 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -387,7 +405,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -409,6 +427,20 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="60.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Placing of drc in the index_return position is added.
</commit_message>
<xml_diff>
--- a/All_rules.xlsx
+++ b/All_rules.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Rule</t>
   </si>
@@ -161,11 +161,31 @@
 errorLayer(L83789 "OXIDE.W.2.1.2: 2.5V N-channel gate width must be &gt;= 0.15 um")</t>
   </si>
   <si>
-    <t>
+    <t>and L512 Poly L94841;
+edge_boolean -inside Oxide L94841 L43550;
 rule OXIDE.W.2.1.2 {
     caption OXIDE.W.2.1.2: Minimum 1.8V N-channel gate width &gt;= 0.32 um;
     inte L43550 L43550 -lt 0.32 -output region -abut lt 90;
 }</t>
+  </si>
+  <si>
+    <t>METAL1.L.1</t>
+  </si>
+  <si>
+    <t>L51265=geomGetNon90(Metal1)
+L28380=geomGetLength(L51265 keep&lt;0.18)
+errorLayer(L28380
+    "METAL1.L.1: Metal1 non-90 degree segments must be &gt;= 0.18 um")</t>
+  </si>
+  <si>
+    <t>angle Metal1 -ltgt 0 90 L79182;
+Rule METAL1.L.1 {
+    caption METAL1.L.1: Metal1 non-90 degree segments must be &gt;= 0.1 um;
+    edge_length L79182 -lt 0.1;
+}</t>
+  </si>
+  <si>
+    <t>L51265 repeated four times. So the rule must be printed outside the rule</t>
   </si>
 </sst>
 </file>
@@ -175,7 +195,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -209,11 +229,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -258,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,10 +295,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,12 +315,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -334,7 +345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="60.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -348,7 +359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="107.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -362,7 +373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="72.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -404,7 +415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -432,8 +443,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="60.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+    <row r="9" customFormat="false" ht="95.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -441,6 +452,21 @@
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="D9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="100.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>